<commit_message>
Updated the Marriage Expense Sheet
</commit_message>
<xml_diff>
--- a/Information/Expenses/Marriage_2019_02_18/Expenses/Expenses_Estimate_Marriage_Till_March_2019_01_08.xlsx
+++ b/Information/Expenses/Marriage_2019_02_18/Expenses/Expenses_Estimate_Marriage_Till_March_2019_01_08.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Engagement_Expenses" sheetId="1" state="visible" r:id="rId2"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="89">
   <si>
     <t xml:space="preserve">Date</t>
   </si>
@@ -133,11 +133,43 @@
     <t xml:space="preserve">Already Saved Money from Salary</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="FreeMono"/>
+        <family val="3"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">9</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="12"/>
+        <rFont val="FreeMono"/>
+        <family val="3"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">th</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="FreeMono"/>
+        <family val="3"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> January</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Transferred for Buying Dresses</t>
+  </si>
+  <si>
     <t xml:space="preserve">Yet to Transfer</t>
   </si>
   <si>
-    <t xml:space="preserve">Before 12th Jan – 50000 
-Before 20th Jan – 150000</t>
+    <t xml:space="preserve">Before 20th Jan – 150000</t>
   </si>
   <si>
     <t xml:space="preserve">Plan is to only Transfer 200000 and Let her manage with it.  
@@ -322,6 +354,56 @@
   </si>
   <si>
     <t xml:space="preserve">To Transfer Amma</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="FreeMono"/>
+        <family val="3"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">50k on 9</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="12"/>
+        <rFont val="FreeMono"/>
+        <family val="3"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">th</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="FreeMono"/>
+        <family val="3"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> Jan
+1.5L to be transferred before 20</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="12"/>
+        <rFont val="FreeMono"/>
+        <family val="3"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">th</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="FreeMono"/>
+        <family val="3"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> Jan</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">To Pay PG</t>
@@ -1224,10 +1306,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A4:E9"/>
+  <dimension ref="A4:E10"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D5" activeCellId="0" sqref="D5"/>
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E10" activeCellId="0" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1236,7 +1318,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="5" width="22.36"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="5" width="42.82"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="5" width="50.27"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="6" width="24.24"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="6" width="24.23"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="6" style="5" width="11.52"/>
   </cols>
   <sheetData>
@@ -1279,18 +1361,32 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="197.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B9" s="10" t="s">
         <v>9</v>
       </c>
       <c r="C9" s="11" t="n">
+        <v>50000</v>
+      </c>
+      <c r="D9" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="E9" s="12" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="192.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B10" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="C10" s="11" t="n">
         <v>250000</v>
       </c>
-      <c r="D9" s="13" t="s">
-        <v>10</v>
-      </c>
-      <c r="E9" s="12" t="s">
-        <v>11</v>
+      <c r="D10" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="E10" s="12" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -1311,13 +1407,13 @@
   </sheetPr>
   <dimension ref="A3:AMJ64"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B24" activeCellId="0" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="5" width="13.01"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="5" width="13.02"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="6" width="57.72"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="6" width="45.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="6" width="35.89"/>
@@ -1327,10 +1423,10 @@
   <sheetData>
     <row r="3" customFormat="false" ht="18.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="2" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>5</v>
@@ -1338,128 +1434,128 @@
     </row>
     <row r="4" customFormat="false" ht="37.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="13" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C4" s="13" t="n">
         <v>25000</v>
       </c>
       <c r="D4" s="13" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B5" s="13" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C5" s="13" t="n">
         <v>20000</v>
       </c>
       <c r="D5" s="13" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B6" s="13" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C6" s="13" t="n">
         <v>120000</v>
       </c>
       <c r="D6" s="13" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="37.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B7" s="13" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C7" s="13" t="n">
         <v>18000</v>
       </c>
       <c r="D7" s="13" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="49.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B8" s="13" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C8" s="13" t="n">
         <v>100000</v>
       </c>
       <c r="D8" s="13" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B9" s="13" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C9" s="13" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="D9" s="13"/>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B10" s="13" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C10" s="13" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="D10" s="13"/>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B11" s="13" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="C11" s="13" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="D11" s="13"/>
     </row>
     <row r="12" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B12" s="13" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="C12" s="13" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="D12" s="13"/>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B13" s="13" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C13" s="13" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="D13" s="13"/>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B14" s="13" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="C14" s="13" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="D14" s="13"/>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B15" s="13" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="C15" s="13" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="D15" s="13"/>
     </row>
     <row r="16" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B16" s="13" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="C16" s="13" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="D16" s="13"/>
     </row>
@@ -1470,7 +1566,7 @@
     </row>
     <row r="18" customFormat="false" ht="50.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B18" s="14" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C18" s="14"/>
       <c r="D18" s="14"/>
@@ -1482,21 +1578,21 @@
     </row>
     <row r="21" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B21" s="15" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="C21" s="16" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="D21" s="16" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="E21" s="16" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B22" s="17" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="C22" s="17" t="n">
         <v>120000</v>
@@ -1506,7 +1602,7 @@
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B23" s="17" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C23" s="17" t="n">
         <v>25000</v>
@@ -1514,19 +1610,23 @@
       <c r="D23" s="17"/>
       <c r="E23" s="17"/>
     </row>
-    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" customFormat="false" ht="52.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B24" s="17" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="C24" s="17" t="n">
         <v>200000</v>
       </c>
-      <c r="D24" s="17"/>
-      <c r="E24" s="17"/>
+      <c r="D24" s="17" t="n">
+        <v>50000</v>
+      </c>
+      <c r="E24" s="17" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B25" s="17" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="C25" s="17" t="n">
         <v>2000</v>
@@ -1536,7 +1636,7 @@
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B26" s="17" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="C26" s="17" t="n">
         <v>15000</v>
@@ -1546,7 +1646,7 @@
     </row>
     <row r="27" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B27" s="18" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="C27" s="18" t="n">
         <f aca="false">SUM(C22:C26)</f>
@@ -1557,7 +1657,7 @@
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B28" s="17" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="C28" s="19" t="n">
         <v>25000</v>
@@ -1567,7 +1667,7 @@
     </row>
     <row r="29" customFormat="false" ht="31.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B29" s="20" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="C29" s="20" t="n">
         <f aca="false">C27-C28</f>
@@ -1578,7 +1678,7 @@
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B30" s="17" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="C30" s="17" t="n">
         <v>110000</v>
@@ -1588,7 +1688,7 @@
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B31" s="17" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="C31" s="17" t="n">
         <v>95000</v>
@@ -1598,7 +1698,7 @@
     </row>
     <row r="32" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B32" s="21" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="C32" s="22" t="n">
         <v>205000</v>
@@ -1608,7 +1708,7 @@
     </row>
     <row r="33" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B33" s="23" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="C33" s="23" t="n">
         <f aca="false">C29-C32</f>
@@ -1619,12 +1719,12 @@
     </row>
     <row r="35" customFormat="false" ht="31.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B35" s="24" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B36" s="17" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="C36" s="22" t="n">
         <f aca="false">3500*78</f>
@@ -1635,7 +1735,7 @@
     </row>
     <row r="37" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B37" s="25" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="C37" s="26" t="n">
         <f aca="false">C36-C33</f>
@@ -1646,7 +1746,7 @@
     </row>
     <row r="39" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B39" s="15" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="C39" s="17"/>
       <c r="D39" s="17"/>
@@ -1654,7 +1754,7 @@
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B40" s="17" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="C40" s="17" t="n">
         <v>18000</v>
@@ -1664,7 +1764,7 @@
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B41" s="17" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="C41" s="17" t="n">
         <v>50000</v>
@@ -1674,7 +1774,7 @@
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B42" s="17" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C42" s="17" t="n">
         <v>20000</v>
@@ -1684,7 +1784,7 @@
     </row>
     <row r="43" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B43" s="18" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="C43" s="18" t="n">
         <f aca="false">SUM(C40:C42)</f>
@@ -1695,7 +1795,7 @@
     </row>
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B44" s="17" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="C44" s="19" t="n">
         <v>0</v>
@@ -1706,7 +1806,7 @@
     <row r="45" customFormat="false" ht="31.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0"/>
       <c r="B45" s="20" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="C45" s="20" t="n">
         <f aca="false">C43-C44</f>
@@ -2736,7 +2836,7 @@
     </row>
     <row r="46" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B46" s="25" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="C46" s="26" t="n">
         <f aca="false">C37-13000</f>
@@ -2747,7 +2847,7 @@
     </row>
     <row r="47" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B47" s="21" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="C47" s="22" t="n">
         <f aca="false">C46</f>
@@ -2758,7 +2858,7 @@
     </row>
     <row r="48" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B48" s="23" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="C48" s="23" t="n">
         <f aca="false">C45-C47</f>
@@ -2769,17 +2869,17 @@
     </row>
     <row r="50" customFormat="false" ht="31.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B50" s="24" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B51" s="17" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B53" s="15" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="C53" s="17"/>
       <c r="D53" s="17"/>
@@ -2787,7 +2887,7 @@
     </row>
     <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B54" s="17" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="C54" s="17" t="n">
         <v>100000</v>
@@ -2797,7 +2897,7 @@
     </row>
     <row r="55" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B55" s="18" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="C55" s="18" t="n">
         <f aca="false">SUM(C54:C54)</f>
@@ -2808,7 +2908,7 @@
     </row>
     <row r="56" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B56" s="17" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="C56" s="19" t="n">
         <v>50000</v>
@@ -2818,7 +2918,7 @@
     </row>
     <row r="57" customFormat="false" ht="31.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B57" s="20" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="C57" s="20" t="n">
         <f aca="false">C55-C56</f>
@@ -2829,7 +2929,7 @@
     </row>
     <row r="58" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B58" s="25" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="C58" s="26" t="n">
         <f aca="false">-C48-15000</f>
@@ -2840,7 +2940,7 @@
     </row>
     <row r="59" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B59" s="17" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="C59" s="17" t="n">
         <v>200000</v>
@@ -2850,7 +2950,7 @@
     </row>
     <row r="60" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B60" s="21" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="C60" s="22" t="n">
         <f aca="false">C59+C58</f>
@@ -2861,7 +2961,7 @@
     </row>
     <row r="61" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B61" s="23" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="C61" s="23" t="n">
         <f aca="false">C57-C60</f>
@@ -2872,12 +2972,12 @@
     </row>
     <row r="63" customFormat="false" ht="31.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B63" s="24" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B64" s="17" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
     </row>
   </sheetData>
@@ -2914,16 +3014,16 @@
   <sheetData>
     <row r="1" customFormat="false" ht="18.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="27" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="B1" s="27"/>
     </row>
     <row r="3" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="28" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="B3" s="28" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2932,37 +3032,37 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="29" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="B5" s="29"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="29" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="B6" s="29"/>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="29" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="B7" s="29"/>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="29" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="B8" s="29"/>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="29" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="B9" s="29"/>
     </row>
     <row r="10" customFormat="false" ht="31.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="20" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="B10" s="29"/>
     </row>
@@ -2972,43 +3072,43 @@
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="29" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="B12" s="29"/>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="29" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="B13" s="29"/>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="29" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="B14" s="29"/>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="29" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="B15" s="29"/>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="29" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="B16" s="29"/>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="29" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="B17" s="29"/>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="29" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="B18" s="29"/>
     </row>
@@ -3018,7 +3118,7 @@
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="29" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="B20" s="29"/>
     </row>

</xml_diff>

<commit_message>
Updated the Marriage Expenses Sheet
</commit_message>
<xml_diff>
--- a/Information/Expenses/Marriage_2019_02_18/Expenses/Expenses_Estimate_Marriage_Till_March_2019_01_08.xlsx
+++ b/Information/Expenses/Marriage_2019_02_18/Expenses/Expenses_Estimate_Marriage_Till_March_2019_01_08.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="98">
   <si>
     <t xml:space="preserve">Date</t>
   </si>
@@ -245,12 +245,18 @@
     <t xml:space="preserve">Manage with the Existing T Shirts</t>
   </si>
   <si>
+    <t xml:space="preserve">Some color Polo T Shirts May be Required</t>
+  </si>
+  <si>
     <t xml:space="preserve">Shirts</t>
   </si>
   <si>
     <t xml:space="preserve">Manage with the Existing Shirts</t>
   </si>
   <si>
+    <t xml:space="preserve">1 More Additional Shirt Required</t>
+  </si>
+  <si>
     <t xml:space="preserve">Jeans</t>
   </si>
   <si>
@@ -263,18 +269,27 @@
     <t xml:space="preserve">Manage with the Existing Track Pants</t>
   </si>
   <si>
+    <t xml:space="preserve">Manage with the Existing ones. Tk more Dhoti</t>
+  </si>
+  <si>
     <t xml:space="preserve">Inners</t>
   </si>
   <si>
     <t xml:space="preserve">Manage with the Existing Inners</t>
   </si>
   <si>
+    <t xml:space="preserve">Buy some Tight Inners as you may be staying in a Different Place. All in Black</t>
+  </si>
+  <si>
     <t xml:space="preserve">Lungi/Dhoti</t>
   </si>
   <si>
     <t xml:space="preserve">Manage with the Existing Ones</t>
   </si>
   <si>
+    <t xml:space="preserve">Tk more Dhotis</t>
+  </si>
+  <si>
     <t xml:space="preserve">Slippers</t>
   </si>
   <si>
@@ -282,6 +297,12 @@
   </si>
   <si>
     <t xml:space="preserve">Manage with the One Bought From Germany</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Formal Socks</t>
+  </si>
+  <si>
+    <t xml:space="preserve">To Buy a Pair</t>
   </si>
   <si>
     <r>
@@ -383,7 +404,7 @@
         <charset val="1"/>
       </rPr>
       <t xml:space="preserve"> Jan
-1.5L to be transferred before 20</t>
+1L on 20</t>
     </r>
     <r>
       <rPr>
@@ -402,7 +423,27 @@
         <family val="3"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve"> Jan</t>
+      <t xml:space="preserve"> Jan
+75k to be transferred on 1</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="12"/>
+        <rFont val="FreeMono"/>
+        <family val="3"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">st</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="FreeMono"/>
+        <family val="3"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> Week of Feb</t>
     </r>
   </si>
   <si>
@@ -410,6 +451,9 @@
   </si>
   <si>
     <t xml:space="preserve">To Buy Minimal Things for the Apartment</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Can be Paid Via Credit Card</t>
   </si>
   <si>
     <t xml:space="preserve">Amount to Have</t>
@@ -458,7 +502,7 @@
         <family val="3"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">Current Balance on 8</t>
+      <t xml:space="preserve">Current Balance on 20</t>
     </r>
     <r>
       <rPr>
@@ -581,6 +625,36 @@
   </si>
   <si>
     <t xml:space="preserve">Euros</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="FreeMono"/>
+        <family val="3"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">14</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="12"/>
+        <rFont val="FreeMono"/>
+        <family val="3"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">th</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="FreeMono"/>
+        <family val="3"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> Jan – Brunda Exchanged it for me.Love You Brunda :)</t>
+    </r>
   </si>
   <si>
     <r>
@@ -965,7 +1039,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -982,6 +1056,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFFE994"/>
         <bgColor rgb="FFFFDBB6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFAA95"/>
+        <bgColor rgb="FFFFA6A6"/>
       </patternFill>
     </fill>
     <fill>
@@ -1005,7 +1085,7 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFA6A6"/>
-        <bgColor rgb="FFFF8080"/>
+        <bgColor rgb="FFFFAA95"/>
       </patternFill>
     </fill>
     <fill>
@@ -1062,7 +1142,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="31">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1119,11 +1199,15 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="8" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1143,19 +1227,15 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="9" fillId="6" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="6" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="7" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="7" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="11" fillId="7" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1167,7 +1247,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="9" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="10" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="10" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1175,7 +1259,7 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="6" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1215,7 +1299,7 @@
       <rgbColor rgb="FFFFFFCC"/>
       <rgbColor rgb="FFCCFFFF"/>
       <rgbColor rgb="FF660066"/>
-      <rgbColor rgb="FFFF8080"/>
+      <rgbColor rgb="FFFFAA95"/>
       <rgbColor rgb="FF0066CC"/>
       <rgbColor rgb="FFCCCCFF"/>
       <rgbColor rgb="FF000080"/>
@@ -1308,8 +1392,8 @@
   </sheetPr>
   <dimension ref="A4:E10"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E10" activeCellId="0" sqref="E10"/>
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C8" activeCellId="0" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1318,7 +1402,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="5" width="22.36"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="5" width="42.82"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="5" width="50.27"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="6" width="24.23"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="6" width="24.22"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="6" style="5" width="11.52"/>
   </cols>
   <sheetData>
@@ -1407,8 +1491,8 @@
   </sheetPr>
   <dimension ref="A3:AMJ64"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B24" activeCellId="0" sqref="B24"/>
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1487,89 +1571,103 @@
         <v>25</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="25.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B9" s="13" t="s">
         <v>26</v>
       </c>
       <c r="C9" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="D9" s="13"/>
-    </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D9" s="14" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="25.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B10" s="13" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C10" s="13" t="s">
-        <v>29</v>
-      </c>
-      <c r="D10" s="13"/>
+        <v>30</v>
+      </c>
+      <c r="D10" s="14" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B11" s="13" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="C11" s="13" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="D11" s="13"/>
     </row>
     <row r="12" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B12" s="13" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C12" s="13" t="s">
-        <v>33</v>
-      </c>
-      <c r="D12" s="13"/>
-    </row>
-    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>35</v>
+      </c>
+      <c r="D12" s="13" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="49.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B13" s="13" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="C13" s="13" t="s">
-        <v>35</v>
-      </c>
-      <c r="D13" s="13"/>
+        <v>38</v>
+      </c>
+      <c r="D13" s="13" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B14" s="13" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="C14" s="13" t="s">
-        <v>37</v>
-      </c>
-      <c r="D14" s="13"/>
+        <v>41</v>
+      </c>
+      <c r="D14" s="13" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B15" s="13" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="C15" s="13" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="D15" s="13"/>
     </row>
     <row r="16" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B16" s="13" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="C16" s="13" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="D16" s="13"/>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B17" s="13"/>
+      <c r="B17" s="13" t="s">
+        <v>46</v>
+      </c>
       <c r="C17" s="13"/>
-      <c r="D17" s="13"/>
+      <c r="D17" s="13" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="18" customFormat="false" ht="50.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B18" s="14" t="s">
-        <v>41</v>
-      </c>
-      <c r="C18" s="14"/>
-      <c r="D18" s="14"/>
+      <c r="B18" s="15" t="s">
+        <v>48</v>
+      </c>
+      <c r="C18" s="15"/>
+      <c r="D18" s="15"/>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B19" s="13"/>
@@ -1577,243 +1675,250 @@
       <c r="D19" s="13"/>
     </row>
     <row r="21" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B21" s="15" t="s">
-        <v>42</v>
-      </c>
-      <c r="C21" s="16" t="s">
-        <v>43</v>
-      </c>
-      <c r="D21" s="16" t="s">
-        <v>44</v>
-      </c>
-      <c r="E21" s="16" t="s">
-        <v>45</v>
+      <c r="B21" s="16" t="s">
+        <v>49</v>
+      </c>
+      <c r="C21" s="17" t="s">
+        <v>50</v>
+      </c>
+      <c r="D21" s="17" t="s">
+        <v>51</v>
+      </c>
+      <c r="E21" s="17" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B22" s="17" t="s">
-        <v>46</v>
-      </c>
-      <c r="C22" s="17" t="n">
+      <c r="B22" s="18" t="s">
+        <v>53</v>
+      </c>
+      <c r="C22" s="18" t="n">
         <v>120000</v>
       </c>
-      <c r="D22" s="17"/>
-      <c r="E22" s="17"/>
+      <c r="D22" s="18"/>
+      <c r="E22" s="18"/>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B23" s="17" t="s">
+      <c r="B23" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="C23" s="17" t="n">
+      <c r="C23" s="18" t="n">
         <v>25000</v>
       </c>
-      <c r="D23" s="17"/>
-      <c r="E23" s="17"/>
-    </row>
-    <row r="24" customFormat="false" ht="52.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B24" s="17" t="s">
-        <v>47</v>
-      </c>
-      <c r="C24" s="17" t="n">
+      <c r="D23" s="18"/>
+      <c r="E23" s="18"/>
+    </row>
+    <row r="24" customFormat="false" ht="77" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B24" s="18" t="s">
+        <v>54</v>
+      </c>
+      <c r="C24" s="18" t="n">
         <v>200000</v>
       </c>
-      <c r="D24" s="17" t="n">
-        <v>50000</v>
-      </c>
-      <c r="E24" s="17" t="s">
-        <v>48</v>
+      <c r="D24" s="18" t="n">
+        <v>150000</v>
+      </c>
+      <c r="E24" s="18" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B25" s="17" t="s">
-        <v>49</v>
-      </c>
-      <c r="C25" s="17" t="n">
+      <c r="B25" s="18" t="s">
+        <v>56</v>
+      </c>
+      <c r="C25" s="18" t="n">
         <v>2000</v>
       </c>
-      <c r="D25" s="17"/>
-      <c r="E25" s="17"/>
-    </row>
-    <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B26" s="17" t="s">
-        <v>50</v>
-      </c>
-      <c r="C26" s="17" t="n">
-        <v>15000</v>
-      </c>
-      <c r="D26" s="17"/>
-      <c r="E26" s="17"/>
+      <c r="D25" s="18"/>
+      <c r="E25" s="18"/>
+    </row>
+    <row r="26" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B26" s="18" t="s">
+        <v>57</v>
+      </c>
+      <c r="C26" s="18" t="n">
+        <v>25000</v>
+      </c>
+      <c r="D26" s="18"/>
+      <c r="E26" s="18" t="s">
+        <v>58</v>
+      </c>
     </row>
     <row r="27" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B27" s="18" t="s">
-        <v>51</v>
-      </c>
-      <c r="C27" s="18" t="n">
+      <c r="B27" s="19" t="s">
+        <v>59</v>
+      </c>
+      <c r="C27" s="19" t="n">
         <f aca="false">SUM(C22:C26)</f>
-        <v>362000</v>
-      </c>
-      <c r="D27" s="18"/>
-      <c r="E27" s="18"/>
+        <v>372000</v>
+      </c>
+      <c r="D27" s="19"/>
+      <c r="E27" s="19"/>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B28" s="17" t="s">
-        <v>52</v>
-      </c>
-      <c r="C28" s="19" t="n">
-        <v>25000</v>
-      </c>
-      <c r="D28" s="19"/>
-      <c r="E28" s="19"/>
+      <c r="B28" s="18" t="s">
+        <v>60</v>
+      </c>
+      <c r="C28" s="20" t="n">
+        <v>40000</v>
+      </c>
+      <c r="D28" s="20"/>
+      <c r="E28" s="20"/>
     </row>
     <row r="29" customFormat="false" ht="31.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B29" s="20" t="s">
-        <v>53</v>
-      </c>
-      <c r="C29" s="20" t="n">
+      <c r="B29" s="21" t="s">
+        <v>61</v>
+      </c>
+      <c r="C29" s="21" t="n">
         <f aca="false">C27-C28</f>
-        <v>337000</v>
-      </c>
-      <c r="D29" s="20"/>
-      <c r="E29" s="20"/>
+        <v>332000</v>
+      </c>
+      <c r="D29" s="21"/>
+      <c r="E29" s="21"/>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B30" s="17" t="s">
-        <v>54</v>
-      </c>
-      <c r="C30" s="17" t="n">
-        <v>110000</v>
-      </c>
-      <c r="D30" s="17"/>
-      <c r="E30" s="17"/>
+      <c r="B30" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="C30" s="18" t="n">
+        <v>251000</v>
+      </c>
+      <c r="D30" s="18"/>
+      <c r="E30" s="18"/>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B31" s="17" t="s">
-        <v>55</v>
-      </c>
-      <c r="C31" s="17" t="n">
+      <c r="B31" s="18" t="s">
+        <v>63</v>
+      </c>
+      <c r="C31" s="18" t="n">
         <v>95000</v>
       </c>
-      <c r="D31" s="17"/>
-      <c r="E31" s="17"/>
+      <c r="D31" s="18"/>
+      <c r="E31" s="18"/>
     </row>
     <row r="32" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B32" s="21" t="s">
-        <v>56</v>
-      </c>
-      <c r="C32" s="22" t="n">
-        <v>205000</v>
-      </c>
-      <c r="D32" s="22"/>
-      <c r="E32" s="22"/>
+      <c r="B32" s="22" t="s">
+        <v>64</v>
+      </c>
+      <c r="C32" s="23" t="n">
+        <f aca="false">C30+C31</f>
+        <v>346000</v>
+      </c>
+      <c r="D32" s="23"/>
+      <c r="E32" s="23"/>
     </row>
     <row r="33" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B33" s="23" t="s">
-        <v>57</v>
-      </c>
-      <c r="C33" s="23" t="n">
+      <c r="B33" s="24" t="s">
+        <v>65</v>
+      </c>
+      <c r="C33" s="24" t="n">
         <f aca="false">C29-C32</f>
-        <v>132000</v>
-      </c>
-      <c r="D33" s="23"/>
-      <c r="E33" s="23"/>
+        <v>-14000</v>
+      </c>
+      <c r="D33" s="24"/>
+      <c r="E33" s="24"/>
     </row>
     <row r="35" customFormat="false" ht="31.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B35" s="24" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="36" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B36" s="17" t="s">
-        <v>59</v>
-      </c>
-      <c r="C36" s="22" t="n">
+      <c r="B35" s="25" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="51.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B36" s="18" t="s">
+        <v>67</v>
+      </c>
+      <c r="C36" s="23" t="n">
         <f aca="false">3500*78</f>
         <v>273000</v>
       </c>
-      <c r="D36" s="22"/>
-      <c r="E36" s="22"/>
+      <c r="D36" s="23" t="n">
+        <v>287567</v>
+      </c>
+      <c r="E36" s="18" t="s">
+        <v>68</v>
+      </c>
     </row>
     <row r="37" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B37" s="25" t="s">
-        <v>60</v>
-      </c>
-      <c r="C37" s="26" t="n">
+      <c r="B37" s="26" t="s">
+        <v>69</v>
+      </c>
+      <c r="C37" s="27" t="n">
         <f aca="false">C36-C33</f>
-        <v>141000</v>
-      </c>
-      <c r="D37" s="26"/>
-      <c r="E37" s="26"/>
+        <v>287000</v>
+      </c>
+      <c r="D37" s="27"/>
+      <c r="E37" s="27"/>
     </row>
     <row r="39" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B39" s="15" t="s">
-        <v>61</v>
-      </c>
-      <c r="C39" s="17"/>
-      <c r="D39" s="17"/>
-      <c r="E39" s="17"/>
+      <c r="B39" s="16" t="s">
+        <v>70</v>
+      </c>
+      <c r="C39" s="18"/>
+      <c r="D39" s="18"/>
+      <c r="E39" s="18"/>
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B40" s="17" t="s">
-        <v>62</v>
-      </c>
-      <c r="C40" s="17" t="n">
+      <c r="B40" s="18" t="s">
+        <v>71</v>
+      </c>
+      <c r="C40" s="18" t="n">
         <v>18000</v>
       </c>
-      <c r="D40" s="17"/>
-      <c r="E40" s="17"/>
+      <c r="D40" s="18"/>
+      <c r="E40" s="18"/>
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B41" s="17" t="s">
-        <v>47</v>
-      </c>
-      <c r="C41" s="17" t="n">
+      <c r="B41" s="18" t="s">
+        <v>54</v>
+      </c>
+      <c r="C41" s="18" t="n">
         <v>50000</v>
       </c>
-      <c r="D41" s="17"/>
-      <c r="E41" s="17"/>
+      <c r="D41" s="18"/>
+      <c r="E41" s="18"/>
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B42" s="17" t="s">
+      <c r="B42" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="C42" s="17" t="n">
+      <c r="C42" s="18" t="n">
         <v>20000</v>
       </c>
-      <c r="D42" s="17"/>
-      <c r="E42" s="17"/>
+      <c r="D42" s="18"/>
+      <c r="E42" s="18"/>
     </row>
     <row r="43" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B43" s="18" t="s">
-        <v>51</v>
-      </c>
-      <c r="C43" s="18" t="n">
+      <c r="B43" s="19" t="s">
+        <v>59</v>
+      </c>
+      <c r="C43" s="19" t="n">
         <f aca="false">SUM(C40:C42)</f>
         <v>88000</v>
       </c>
-      <c r="D43" s="18"/>
-      <c r="E43" s="18"/>
+      <c r="D43" s="19"/>
+      <c r="E43" s="19"/>
     </row>
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B44" s="17" t="s">
-        <v>52</v>
-      </c>
-      <c r="C44" s="19" t="n">
+      <c r="B44" s="18" t="s">
+        <v>60</v>
+      </c>
+      <c r="C44" s="20" t="n">
         <v>0</v>
       </c>
-      <c r="D44" s="19"/>
-      <c r="E44" s="19"/>
+      <c r="D44" s="20"/>
+      <c r="E44" s="20"/>
     </row>
     <row r="45" customFormat="false" ht="31.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0"/>
-      <c r="B45" s="20" t="s">
-        <v>53</v>
-      </c>
-      <c r="C45" s="20" t="n">
+      <c r="B45" s="21" t="s">
+        <v>61</v>
+      </c>
+      <c r="C45" s="21" t="n">
         <f aca="false">C43-C44</f>
         <v>88000</v>
       </c>
-      <c r="D45" s="20"/>
-      <c r="E45" s="20"/>
+      <c r="D45" s="21"/>
+      <c r="E45" s="21"/>
       <c r="F45" s="0"/>
       <c r="G45" s="0"/>
       <c r="H45" s="0"/>
@@ -2835,149 +2940,149 @@
       <c r="AMJ45" s="0"/>
     </row>
     <row r="46" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B46" s="25" t="s">
-        <v>63</v>
-      </c>
-      <c r="C46" s="26" t="n">
+      <c r="B46" s="26" t="s">
+        <v>72</v>
+      </c>
+      <c r="C46" s="27" t="n">
         <f aca="false">C37-13000</f>
-        <v>128000</v>
-      </c>
-      <c r="D46" s="26"/>
-      <c r="E46" s="26"/>
+        <v>274000</v>
+      </c>
+      <c r="D46" s="27"/>
+      <c r="E46" s="27"/>
     </row>
     <row r="47" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B47" s="21" t="s">
-        <v>56</v>
-      </c>
-      <c r="C47" s="22" t="n">
+      <c r="B47" s="22" t="s">
+        <v>64</v>
+      </c>
+      <c r="C47" s="23" t="n">
         <f aca="false">C46</f>
-        <v>128000</v>
-      </c>
-      <c r="D47" s="22"/>
-      <c r="E47" s="22"/>
+        <v>274000</v>
+      </c>
+      <c r="D47" s="23"/>
+      <c r="E47" s="23"/>
     </row>
     <row r="48" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B48" s="23" t="s">
-        <v>57</v>
-      </c>
-      <c r="C48" s="23" t="n">
+      <c r="B48" s="24" t="s">
+        <v>65</v>
+      </c>
+      <c r="C48" s="24" t="n">
         <f aca="false">C45-C47</f>
-        <v>-40000</v>
-      </c>
-      <c r="D48" s="23"/>
-      <c r="E48" s="23"/>
+        <v>-186000</v>
+      </c>
+      <c r="D48" s="24"/>
+      <c r="E48" s="24"/>
     </row>
     <row r="50" customFormat="false" ht="31.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B50" s="24" t="s">
-        <v>64</v>
+      <c r="B50" s="25" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B51" s="17" t="s">
-        <v>65</v>
+      <c r="B51" s="18" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B53" s="15" t="s">
-        <v>66</v>
-      </c>
-      <c r="C53" s="17"/>
-      <c r="D53" s="17"/>
-      <c r="E53" s="17"/>
+      <c r="B53" s="16" t="s">
+        <v>75</v>
+      </c>
+      <c r="C53" s="18"/>
+      <c r="D53" s="18"/>
+      <c r="E53" s="18"/>
     </row>
     <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B54" s="17" t="s">
-        <v>67</v>
-      </c>
-      <c r="C54" s="17" t="n">
+      <c r="B54" s="18" t="s">
+        <v>76</v>
+      </c>
+      <c r="C54" s="18" t="n">
         <v>100000</v>
       </c>
-      <c r="D54" s="17"/>
-      <c r="E54" s="17"/>
+      <c r="D54" s="18"/>
+      <c r="E54" s="18"/>
     </row>
     <row r="55" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B55" s="18" t="s">
-        <v>51</v>
-      </c>
-      <c r="C55" s="18" t="n">
+      <c r="B55" s="19" t="s">
+        <v>59</v>
+      </c>
+      <c r="C55" s="19" t="n">
         <f aca="false">SUM(C54:C54)</f>
         <v>100000</v>
       </c>
-      <c r="D55" s="18"/>
-      <c r="E55" s="18"/>
+      <c r="D55" s="19"/>
+      <c r="E55" s="19"/>
     </row>
     <row r="56" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B56" s="17" t="s">
-        <v>52</v>
-      </c>
-      <c r="C56" s="19" t="n">
+      <c r="B56" s="18" t="s">
+        <v>60</v>
+      </c>
+      <c r="C56" s="20" t="n">
         <v>50000</v>
       </c>
-      <c r="D56" s="19"/>
-      <c r="E56" s="19"/>
+      <c r="D56" s="20"/>
+      <c r="E56" s="20"/>
     </row>
     <row r="57" customFormat="false" ht="31.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B57" s="20" t="s">
-        <v>53</v>
-      </c>
-      <c r="C57" s="20" t="n">
+      <c r="B57" s="21" t="s">
+        <v>61</v>
+      </c>
+      <c r="C57" s="21" t="n">
         <f aca="false">C55-C56</f>
         <v>50000</v>
       </c>
-      <c r="D57" s="20"/>
-      <c r="E57" s="20"/>
+      <c r="D57" s="21"/>
+      <c r="E57" s="21"/>
     </row>
     <row r="58" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B58" s="25" t="s">
-        <v>68</v>
-      </c>
-      <c r="C58" s="26" t="n">
+      <c r="B58" s="26" t="s">
+        <v>77</v>
+      </c>
+      <c r="C58" s="27" t="n">
         <f aca="false">-C48-15000</f>
-        <v>25000</v>
-      </c>
-      <c r="D58" s="26"/>
-      <c r="E58" s="26"/>
+        <v>171000</v>
+      </c>
+      <c r="D58" s="27"/>
+      <c r="E58" s="27"/>
     </row>
     <row r="59" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B59" s="17" t="s">
-        <v>69</v>
-      </c>
-      <c r="C59" s="17" t="n">
+      <c r="B59" s="18" t="s">
+        <v>78</v>
+      </c>
+      <c r="C59" s="18" t="n">
         <v>200000</v>
       </c>
-      <c r="D59" s="17"/>
-      <c r="E59" s="17"/>
+      <c r="D59" s="18"/>
+      <c r="E59" s="18"/>
     </row>
     <row r="60" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B60" s="21" t="s">
-        <v>70</v>
-      </c>
-      <c r="C60" s="22" t="n">
+      <c r="B60" s="22" t="s">
+        <v>79</v>
+      </c>
+      <c r="C60" s="23" t="n">
         <f aca="false">C59+C58</f>
-        <v>225000</v>
-      </c>
-      <c r="D60" s="22"/>
-      <c r="E60" s="22"/>
+        <v>371000</v>
+      </c>
+      <c r="D60" s="23"/>
+      <c r="E60" s="23"/>
     </row>
     <row r="61" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B61" s="23" t="s">
-        <v>57</v>
-      </c>
-      <c r="C61" s="23" t="n">
+      <c r="B61" s="24" t="s">
+        <v>65</v>
+      </c>
+      <c r="C61" s="24" t="n">
         <f aca="false">C57-C60</f>
-        <v>-175000</v>
-      </c>
-      <c r="D61" s="23"/>
-      <c r="E61" s="23"/>
+        <v>-321000</v>
+      </c>
+      <c r="D61" s="24"/>
+      <c r="E61" s="24"/>
     </row>
     <row r="63" customFormat="false" ht="31.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B63" s="24" t="s">
-        <v>71</v>
+      <c r="B63" s="25" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B64" s="17" t="s">
-        <v>65</v>
+      <c r="B64" s="18" t="s">
+        <v>74</v>
       </c>
     </row>
   </sheetData>
@@ -3002,7 +3107,7 @@
   <dimension ref="A1:B20"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3013,114 +3118,114 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="18.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="27" t="s">
-        <v>72</v>
-      </c>
-      <c r="B1" s="27"/>
+      <c r="A1" s="28" t="s">
+        <v>81</v>
+      </c>
+      <c r="B1" s="28"/>
     </row>
     <row r="3" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="28" t="s">
-        <v>73</v>
-      </c>
-      <c r="B3" s="28" t="s">
-        <v>74</v>
+      <c r="A3" s="29" t="s">
+        <v>82</v>
+      </c>
+      <c r="B3" s="29" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="29"/>
-      <c r="B4" s="29"/>
+      <c r="A4" s="30"/>
+      <c r="B4" s="30"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="29" t="s">
-        <v>75</v>
-      </c>
-      <c r="B5" s="29"/>
+      <c r="A5" s="30" t="s">
+        <v>84</v>
+      </c>
+      <c r="B5" s="30"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="29" t="s">
-        <v>76</v>
-      </c>
-      <c r="B6" s="29"/>
+      <c r="A6" s="30" t="s">
+        <v>85</v>
+      </c>
+      <c r="B6" s="30"/>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="29" t="s">
-        <v>77</v>
-      </c>
-      <c r="B7" s="29"/>
+      <c r="A7" s="30" t="s">
+        <v>86</v>
+      </c>
+      <c r="B7" s="30"/>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="29" t="s">
-        <v>78</v>
-      </c>
-      <c r="B8" s="29"/>
+      <c r="A8" s="30" t="s">
+        <v>87</v>
+      </c>
+      <c r="B8" s="30"/>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="29" t="s">
-        <v>79</v>
-      </c>
-      <c r="B9" s="29"/>
+      <c r="A9" s="30" t="s">
+        <v>88</v>
+      </c>
+      <c r="B9" s="30"/>
     </row>
     <row r="10" customFormat="false" ht="31.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="20" t="s">
-        <v>80</v>
-      </c>
-      <c r="B10" s="29"/>
+      <c r="A10" s="21" t="s">
+        <v>89</v>
+      </c>
+      <c r="B10" s="30"/>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="29"/>
-      <c r="B11" s="29"/>
+      <c r="A11" s="30"/>
+      <c r="B11" s="30"/>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="29" t="s">
-        <v>81</v>
-      </c>
-      <c r="B12" s="29"/>
+      <c r="A12" s="30" t="s">
+        <v>90</v>
+      </c>
+      <c r="B12" s="30"/>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="29" t="s">
-        <v>82</v>
-      </c>
-      <c r="B13" s="29"/>
+      <c r="A13" s="30" t="s">
+        <v>91</v>
+      </c>
+      <c r="B13" s="30"/>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="29" t="s">
-        <v>83</v>
-      </c>
-      <c r="B14" s="29"/>
+      <c r="A14" s="30" t="s">
+        <v>92</v>
+      </c>
+      <c r="B14" s="30"/>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="29" t="s">
-        <v>84</v>
-      </c>
-      <c r="B15" s="29"/>
+      <c r="A15" s="30" t="s">
+        <v>93</v>
+      </c>
+      <c r="B15" s="30"/>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="29" t="s">
-        <v>85</v>
-      </c>
-      <c r="B16" s="29"/>
+      <c r="A16" s="30" t="s">
+        <v>94</v>
+      </c>
+      <c r="B16" s="30"/>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="29" t="s">
-        <v>86</v>
-      </c>
-      <c r="B17" s="29"/>
+      <c r="A17" s="30" t="s">
+        <v>95</v>
+      </c>
+      <c r="B17" s="30"/>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="29" t="s">
-        <v>87</v>
-      </c>
-      <c r="B18" s="29"/>
+      <c r="A18" s="30" t="s">
+        <v>96</v>
+      </c>
+      <c r="B18" s="30"/>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="29"/>
-      <c r="B19" s="29"/>
+      <c r="A19" s="30"/>
+      <c r="B19" s="30"/>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="29" t="s">
-        <v>88</v>
-      </c>
-      <c r="B20" s="29"/>
+      <c r="A20" s="30" t="s">
+        <v>97</v>
+      </c>
+      <c r="B20" s="30"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
Updated the Expenses Sheet
</commit_message>
<xml_diff>
--- a/Information/Expenses/Marriage_2019_02_18/Expenses/Expenses_Estimate_Marriage_Till_March_2019_01_08.xlsx
+++ b/Information/Expenses/Marriage_2019_02_18/Expenses/Expenses_Estimate_Marriage_Till_March_2019_01_08.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="101">
   <si>
     <t xml:space="preserve">Date</t>
   </si>
@@ -263,6 +263,9 @@
     <t xml:space="preserve">Manage with the Existing Jeans</t>
   </si>
   <si>
+    <t xml:space="preserve">Bought 4 New Jeans for 6k Rupees</t>
+  </si>
+  <si>
     <t xml:space="preserve">Track Pants</t>
   </si>
   <si>
@@ -297,6 +300,9 @@
   </si>
   <si>
     <t xml:space="preserve">Manage with the One Bought From Germany</t>
+  </si>
+  <si>
+    <t xml:space="preserve">To investigate on the Existing Pair</t>
   </si>
   <si>
     <t xml:space="preserve">Formal Socks</t>
@@ -372,6 +378,36 @@
   </si>
   <si>
     <t xml:space="preserve">House Advance</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="FreeMono"/>
+        <family val="3"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">21</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="12"/>
+        <rFont val="FreeMono"/>
+        <family val="3"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">st</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="FreeMono"/>
+        <family val="3"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> Jan , Credit Card</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">To Transfer Amma</t>
@@ -1347,7 +1383,7 @@
   <dimension ref="B3:C4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
+      <selection pane="topLeft" activeCell="C3" activeCellId="1" sqref="C22:D28 C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1393,7 +1429,7 @@
   <dimension ref="A4:E10"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C8" activeCellId="0" sqref="C8"/>
+      <selection pane="topLeft" activeCell="C8" activeCellId="1" sqref="C22:D28 C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1491,8 +1527,8 @@
   </sheetPr>
   <dimension ref="A3:AMJ64"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A19" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C22" activeCellId="0" sqref="C22:D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1593,78 +1629,82 @@
         <v>31</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B11" s="13" t="s">
         <v>32</v>
       </c>
       <c r="C11" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="D11" s="13"/>
+      <c r="D11" s="13" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="12" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B12" s="13" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C12" s="13" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D12" s="13" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="49.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B13" s="13" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C13" s="13" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D13" s="13" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B14" s="13" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C14" s="13" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D14" s="13" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B15" s="13" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C15" s="13" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D15" s="13"/>
     </row>
     <row r="16" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B16" s="13" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C16" s="13" t="s">
-        <v>45</v>
-      </c>
-      <c r="D16" s="13"/>
+        <v>46</v>
+      </c>
+      <c r="D16" s="13" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B17" s="13" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="C17" s="13"/>
       <c r="D17" s="13" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="50.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B18" s="15" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="C18" s="15"/>
       <c r="D18" s="15"/>
@@ -1676,21 +1716,21 @@
     </row>
     <row r="21" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B21" s="16" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="C21" s="17" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="D21" s="17" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="E21" s="17" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B22" s="18" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C22" s="18" t="n">
         <v>120000</v>
@@ -1698,19 +1738,23 @@
       <c r="D22" s="18"/>
       <c r="E22" s="18"/>
     </row>
-    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" customFormat="false" ht="26.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B23" s="18" t="s">
         <v>16</v>
       </c>
       <c r="C23" s="18" t="n">
         <v>25000</v>
       </c>
-      <c r="D23" s="18"/>
-      <c r="E23" s="18"/>
+      <c r="D23" s="18" t="n">
+        <v>11000</v>
+      </c>
+      <c r="E23" s="18" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="24" customFormat="false" ht="77" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B24" s="18" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="C24" s="18" t="n">
         <v>200000</v>
@@ -1719,12 +1763,12 @@
         <v>150000</v>
       </c>
       <c r="E24" s="18" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B25" s="18" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="C25" s="18" t="n">
         <v>2000</v>
@@ -1734,19 +1778,19 @@
     </row>
     <row r="26" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B26" s="18" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="C26" s="18" t="n">
         <v>25000</v>
       </c>
       <c r="D26" s="18"/>
       <c r="E26" s="18" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B27" s="19" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="C27" s="19" t="n">
         <f aca="false">SUM(C22:C26)</f>
@@ -1757,17 +1801,20 @@
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B28" s="18" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="C28" s="20" t="n">
         <v>40000</v>
       </c>
-      <c r="D28" s="20"/>
+      <c r="D28" s="20" t="n">
+        <f aca="false">D23</f>
+        <v>11000</v>
+      </c>
       <c r="E28" s="20"/>
     </row>
     <row r="29" customFormat="false" ht="31.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B29" s="21" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="C29" s="21" t="n">
         <f aca="false">C27-C28</f>
@@ -1778,7 +1825,7 @@
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B30" s="18" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="C30" s="18" t="n">
         <v>251000</v>
@@ -1788,7 +1835,7 @@
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B31" s="18" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="C31" s="18" t="n">
         <v>95000</v>
@@ -1798,7 +1845,7 @@
     </row>
     <row r="32" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B32" s="22" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="C32" s="23" t="n">
         <f aca="false">C30+C31</f>
@@ -1809,7 +1856,7 @@
     </row>
     <row r="33" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B33" s="24" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="C33" s="24" t="n">
         <f aca="false">C29-C32</f>
@@ -1820,12 +1867,12 @@
     </row>
     <row r="35" customFormat="false" ht="31.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B35" s="25" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="51.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B36" s="18" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="C36" s="23" t="n">
         <f aca="false">3500*78</f>
@@ -1835,12 +1882,12 @@
         <v>287567</v>
       </c>
       <c r="E36" s="18" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B37" s="26" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="C37" s="27" t="n">
         <f aca="false">C36-C33</f>
@@ -1851,7 +1898,7 @@
     </row>
     <row r="39" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B39" s="16" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="C39" s="18"/>
       <c r="D39" s="18"/>
@@ -1859,7 +1906,7 @@
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B40" s="18" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="C40" s="18" t="n">
         <v>18000</v>
@@ -1869,7 +1916,7 @@
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B41" s="18" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="C41" s="18" t="n">
         <v>50000</v>
@@ -1889,7 +1936,7 @@
     </row>
     <row r="43" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B43" s="19" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="C43" s="19" t="n">
         <f aca="false">SUM(C40:C42)</f>
@@ -1900,7 +1947,7 @@
     </row>
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B44" s="18" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="C44" s="20" t="n">
         <v>0</v>
@@ -1911,7 +1958,7 @@
     <row r="45" customFormat="false" ht="31.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0"/>
       <c r="B45" s="21" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="C45" s="21" t="n">
         <f aca="false">C43-C44</f>
@@ -2941,7 +2988,7 @@
     </row>
     <row r="46" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B46" s="26" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="C46" s="27" t="n">
         <f aca="false">C37-13000</f>
@@ -2952,7 +2999,7 @@
     </row>
     <row r="47" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B47" s="22" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="C47" s="23" t="n">
         <f aca="false">C46</f>
@@ -2963,7 +3010,7 @@
     </row>
     <row r="48" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B48" s="24" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="C48" s="24" t="n">
         <f aca="false">C45-C47</f>
@@ -2974,17 +3021,17 @@
     </row>
     <row r="50" customFormat="false" ht="31.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B50" s="25" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B51" s="18" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B53" s="16" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="C53" s="18"/>
       <c r="D53" s="18"/>
@@ -2992,7 +3039,7 @@
     </row>
     <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B54" s="18" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="C54" s="18" t="n">
         <v>100000</v>
@@ -3002,7 +3049,7 @@
     </row>
     <row r="55" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B55" s="19" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="C55" s="19" t="n">
         <f aca="false">SUM(C54:C54)</f>
@@ -3013,7 +3060,7 @@
     </row>
     <row r="56" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B56" s="18" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="C56" s="20" t="n">
         <v>50000</v>
@@ -3023,7 +3070,7 @@
     </row>
     <row r="57" customFormat="false" ht="31.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B57" s="21" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="C57" s="21" t="n">
         <f aca="false">C55-C56</f>
@@ -3034,7 +3081,7 @@
     </row>
     <row r="58" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B58" s="26" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="C58" s="27" t="n">
         <f aca="false">-C48-15000</f>
@@ -3045,7 +3092,7 @@
     </row>
     <row r="59" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B59" s="18" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="C59" s="18" t="n">
         <v>200000</v>
@@ -3055,7 +3102,7 @@
     </row>
     <row r="60" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B60" s="22" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="C60" s="23" t="n">
         <f aca="false">C59+C58</f>
@@ -3066,7 +3113,7 @@
     </row>
     <row r="61" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B61" s="24" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="C61" s="24" t="n">
         <f aca="false">C57-C60</f>
@@ -3077,12 +3124,12 @@
     </row>
     <row r="63" customFormat="false" ht="31.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B63" s="25" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B64" s="18" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
     </row>
   </sheetData>
@@ -3107,7 +3154,7 @@
   <dimension ref="A1:B20"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+      <selection pane="topLeft" activeCell="A3" activeCellId="1" sqref="C22:D28 A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3119,16 +3166,16 @@
   <sheetData>
     <row r="1" customFormat="false" ht="18.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="28" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="B1" s="28"/>
     </row>
     <row r="3" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="29" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="B3" s="29" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3137,37 +3184,37 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="30" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="B5" s="30"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="30" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="B6" s="30"/>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="30" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="B7" s="30"/>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="30" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="B8" s="30"/>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="30" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="B9" s="30"/>
     </row>
     <row r="10" customFormat="false" ht="31.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="21" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="B10" s="30"/>
     </row>
@@ -3177,43 +3224,43 @@
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="30" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="B12" s="30"/>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="30" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="B13" s="30"/>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="30" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="B14" s="30"/>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="30" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="B15" s="30"/>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="30" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="B16" s="30"/>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="30" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="B17" s="30"/>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="30" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="B18" s="30"/>
     </row>
@@ -3223,7 +3270,7 @@
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="30" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="B20" s="30"/>
     </row>

</xml_diff>